<commit_message>
Update Project 2 Work Outline.xlsx
</commit_message>
<xml_diff>
--- a/Project 2 Work Outline.xlsx
+++ b/Project 2 Work Outline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yenja\OneDrive\Documents\2021 Winter\ESSE3670\P2\ESSE3670-Project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C13F72B6-2D5E-4921-BA5B-C604AE908E27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2011DE77-98F2-458F-A318-878CAE169921}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9DB2129D-93F2-4BAD-ACDF-A72AAD50023F}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="9384" xr2:uid="{9DB2129D-93F2-4BAD-ACDF-A72AAD50023F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,10 +68,10 @@
     <t>Write functions that can extract variables from BEF data formats i.e. fixed width and space delimited formats</t>
   </si>
   <si>
-    <t>Write script that takes input data provided, queries for corresponding data structure element from step 2 and computes satellite position using data structure constituents</t>
-  </si>
-  <si>
     <t>Jared</t>
+  </si>
+  <si>
+    <t>Write script that takes input data provided, queries for corresponding data structure element from step 2 and computes satellite position using data structure constituents and outputs values specified by 'Output format.pdf'</t>
   </si>
 </sst>
 </file>
@@ -470,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B122DF0A-C17B-456F-9E48-2FFF20F122EA}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="A1:D5"/>
+      <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +512,7 @@
     </row>
     <row r="3" spans="1:4" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A9" si="0">ROW()-1</f>
+        <f t="shared" ref="A3:A6" si="0">ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -535,10 +535,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="124.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="166.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -547,8 +547,12 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="C6" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Added to Work Outline
</commit_message>
<xml_diff>
--- a/Project 2 Work Outline.xlsx
+++ b/Project 2 Work Outline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yenja\OneDrive\Documents\2021 Winter\ESSE3670\P2\ESSE3670-Project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2011DE77-98F2-458F-A318-878CAE169921}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B4FBCE-567E-4748-AC41-682C193C1B6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="9384" xr2:uid="{9DB2129D-93F2-4BAD-ACDF-A72AAD50023F}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9420" xr2:uid="{9DB2129D-93F2-4BAD-ACDF-A72AAD50023F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Status</t>
   </si>
@@ -71,7 +71,10 @@
     <t>Jared</t>
   </si>
   <si>
-    <t>Write script that takes input data provided, queries for corresponding data structure element from step 2 and computes satellite position using data structure constituents and outputs values specified by 'Output format.pdf'</t>
+    <t xml:space="preserve">Write script that takes input data provided, queries for corresponding data structure element from step 2 </t>
+  </si>
+  <si>
+    <t>Computes satellite position using data structure constituents and outputs values specified by 'Output format.pdf'</t>
   </si>
 </sst>
 </file>
@@ -137,13 +140,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -472,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B122DF0A-C17B-456F-9E48-2FFF20F122EA}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,7 +518,7 @@
     </row>
     <row r="3" spans="1:4" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A6" si="0">ROW()-1</f>
+        <f t="shared" ref="A3:A5" si="0">ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -538,7 +544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="166.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -550,9 +556,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>